<commit_message>
dot improved and Notes added
</commit_message>
<xml_diff>
--- a/imgsolver/model_trainer/model_metric_logs/category_class_v42024-11-09.model.keras_metrics.xlsx
+++ b/imgsolver/model_trainer/model_metric_logs/category_class_v42024-11-09.model.keras_metrics.xlsx
@@ -449,7 +449,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.2720474302768707</v>
+        <v>0.2823184728622437</v>
       </c>
     </row>
     <row r="3">
@@ -459,7 +459,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.9276470541954041</v>
+        <v>0.9249129891395569</v>
       </c>
     </row>
   </sheetData>
@@ -529,16 +529,16 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.9385814793687013</v>
+        <v>0.9303879310344828</v>
       </c>
       <c r="C3" t="n">
-        <v>0.9872</v>
+        <v>0.9853914631362702</v>
       </c>
       <c r="D3" t="n">
-        <v>0.9622770250511746</v>
+        <v>0.9571000997672099</v>
       </c>
       <c r="E3" t="n">
-        <v>5000</v>
+        <v>4381</v>
       </c>
     </row>
     <row r="4">
@@ -567,16 +567,16 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.9276470588235294</v>
+        <v>0.9249130089738111</v>
       </c>
       <c r="C5" t="n">
-        <v>0.9276470588235294</v>
+        <v>0.9249130089738111</v>
       </c>
       <c r="D5" t="n">
-        <v>0.9276470588235294</v>
+        <v>0.9249130089738111</v>
       </c>
       <c r="E5" t="n">
-        <v>0.9276470588235294</v>
+        <v>0.9249130089738111</v>
       </c>
     </row>
     <row r="6">
@@ -586,16 +586,16 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0.8783533823977052</v>
+        <v>0.8756221996196324</v>
       </c>
       <c r="C6" t="n">
-        <v>0.9515333333333333</v>
+        <v>0.95093048771209</v>
       </c>
       <c r="D6" t="n">
-        <v>0.9064557844509132</v>
+        <v>0.9047301426895916</v>
       </c>
       <c r="E6" t="n">
-        <v>17000</v>
+        <v>16381</v>
       </c>
     </row>
     <row r="7">
@@ -605,16 +605,16 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0.9412428481483525</v>
+        <v>0.9391520998437554</v>
       </c>
       <c r="C7" t="n">
-        <v>0.9276470588235294</v>
+        <v>0.9249130089738111</v>
       </c>
       <c r="D7" t="n">
-        <v>0.9300364908568575</v>
+        <v>0.9274336582864814</v>
       </c>
       <c r="E7" t="n">
-        <v>17000</v>
+        <v>16381</v>
       </c>
     </row>
   </sheetData>
@@ -679,7 +679,7 @@
         <v>62</v>
       </c>
       <c r="C3" t="n">
-        <v>4936</v>
+        <v>4317</v>
       </c>
       <c r="D3" t="n">
         <v>2</v>

</xml_diff>